<commit_message>
remove one more space.
</commit_message>
<xml_diff>
--- a/input/sappinfo.xlsx
+++ b/input/sappinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SAPP App\AmiKo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9604699F-5C46-4AB2-AE9A-2DBB66F113E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B198611D-B8F4-4B3B-8E35-88B1236A5D86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="953" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="953" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schwangerschaft" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18264" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18264" uniqueCount="1475">
   <si>
     <t>Indikation</t>
   </si>
@@ -5358,9 +5358,6 @@
   </si>
   <si>
     <t>Piperacillin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> intravenös, peroral</t>
   </si>
   <si>
     <t>nur Einzeldosen, keine Langzeitanwendung</t>
@@ -6026,9 +6023,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AD1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N214" sqref="N214"/>
+    <sheetView topLeftCell="B1" zoomScale="225" zoomScaleNormal="225" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1005" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H661" sqref="H661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -7311,7 +7308,7 @@
         <v>1020</v>
       </c>
       <c r="N21" s="52" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="Y21" s="54"/>
       <c r="Z21" s="53" t="s">
@@ -7357,7 +7354,7 @@
         <v>1020</v>
       </c>
       <c r="N22" s="52" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="Z22" s="53" t="s">
         <v>605</v>
@@ -65589,9 +65586,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V479"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J356" sqref="J356"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A339" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H366" sqref="H366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -75927,7 +75924,7 @@
         <v>734</v>
       </c>
       <c r="H233" s="52" t="s">
-        <v>1474</v>
+        <v>1402</v>
       </c>
       <c r="I233" s="52" t="s">
         <v>1020</v>

</xml_diff>

<commit_message>
new input file for issue #101
</commit_message>
<xml_diff>
--- a/input/sappinfo.xlsx
+++ b/input/sappinfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SAPP App\AmiKo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B198611D-B8F4-4B3B-8E35-88B1236A5D86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E094E414-1543-4E01-93E3-8BAAA4025114}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="953" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="924" yWindow="120" windowWidth="22980" windowHeight="8928" tabRatio="953" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schwangerschaft" sheetId="5" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18264" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18265" uniqueCount="1476">
   <si>
     <t>Indikation</t>
   </si>
@@ -5361,6 +5362,9 @@
   </si>
   <si>
     <t>nur Einzeldosen, keine Langzeitanwendung</t>
+  </si>
+  <si>
+    <t>im 1. Trimenon kontraindiziert</t>
   </si>
 </sst>
 </file>
@@ -6023,9 +6027,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AD1013"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="225" zoomScaleNormal="225" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1005" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H661" sqref="H661"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="225" zoomScaleNormal="225" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A804" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M841" sqref="M841"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -55014,13 +55018,16 @@
         <v>1402</v>
       </c>
       <c r="I831" s="52" t="s">
-        <v>244</v>
+        <v>1393</v>
       </c>
       <c r="J831" s="52" t="s">
         <v>244</v>
       </c>
       <c r="K831" s="52" t="s">
         <v>244</v>
+      </c>
+      <c r="N831" s="52" t="s">
+        <v>1475</v>
       </c>
       <c r="O831" s="7" t="s">
         <v>1343</v>
@@ -65564,13 +65571,13 @@
         <filter val="1"/>
       </filters>
     </filterColumn>
-    <sortState ref="A3:AC1001">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AC1001">
       <sortCondition ref="G2:G1001"/>
       <sortCondition ref="B2:B1001"/>
       <sortCondition ref="C2:C1001"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A5:AD1013">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:AD1013">
     <sortCondition ref="G2:G1013"/>
   </sortState>
   <hyperlinks>
@@ -65586,9 +65593,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A339" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H366" sqref="H366"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G423" sqref="A423:XFD423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -86539,11 +86546,11 @@
         <filter val="1"/>
       </filters>
     </filterColumn>
-    <sortState ref="A5:U479">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:U479">
       <sortCondition ref="G2:G479"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A5:V479">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:V479">
     <sortCondition ref="G2:G479"/>
   </sortState>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>